<commit_message>
Add more sample data.
* Comments were added to each spreadsheet to credit sources.
* Slight readability improvements to codebase.
</commit_message>
<xml_diff>
--- a/data/Data-Contingency-1.xlsx
+++ b/data/Data-Contingency-1.xlsx
@@ -2,15 +2,16 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
+  <fileSharing readOnlyRecommended="1"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kjiwa\PycharmProjects\ee454-power-system-analysis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFCB6E6E-2D0D-4C65-8371-78F594D156BC}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{017F5D4E-C62C-4BDD-839B-5E081501CA65}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{96A0262C-C381-4208-80FC-9B658C6113A4}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{96A0262C-C381-4208-80FC-9B658C6113A4}"/>
   </bookViews>
   <sheets>
     <sheet name="Bus data" sheetId="1" r:id="rId1"/>
@@ -413,7 +414,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C6706C7-AE82-43C4-AF8E-576A594A4AD0}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -596,7 +597,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C31AD803-4839-4A0D-A55F-341A5B575747}">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>

<commit_message>
Fix power ratings for the two lines from bus 1 to 2.
</commit_message>
<xml_diff>
--- a/data/Data-Contingency-1.xlsx
+++ b/data/Data-Contingency-1.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <fileSharing readOnlyRecommended="1"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -9,7 +9,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kjiwa\PycharmProjects\ee454-power-system-analysis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{017F5D4E-C62C-4BDD-839B-5E081501CA65}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA3C5769-FB82-48F3-A368-F16C75FBC722}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{96A0262C-C381-4208-80FC-9B658C6113A4}"/>
   </bookViews>
@@ -638,7 +638,7 @@
         <v>2.64E-2</v>
       </c>
       <c r="F2">
-        <v>95</v>
+        <v>47.5</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>